<commit_message>
trival fix in problem list
</commit_message>
<xml_diff>
--- a/Training/problems solved.xlsx
+++ b/Training/problems solved.xlsx
@@ -290,8 +290,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -390,18 +390,33 @@
   <dimension ref="A2:O18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -469,7 +484,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>43664</v>
       </c>
@@ -488,7 +503,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>43665</v>
       </c>
@@ -507,7 +522,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>43667</v>
       </c>
@@ -526,7 +541,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>43668</v>
       </c>
@@ -545,7 +560,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>43669</v>
       </c>
@@ -564,7 +579,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>43671</v>
       </c>
@@ -583,7 +598,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>43672</v>
       </c>
@@ -602,7 +617,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>43673</v>
       </c>
@@ -621,7 +636,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>43675</v>
       </c>
@@ -640,7 +655,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>43676</v>
       </c>
@@ -659,7 +674,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>43677</v>
       </c>
@@ -697,12 +712,15 @@
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:O2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>